<commit_message>
Updated qc processing to be consistent with CF protocols
</commit_message>
<xml_diff>
--- a/metadata/kt_metadata.xlsx
+++ b/metadata/kt_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heather/Desktop/ace-ceda-master/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F2BDFC-9D8E-6042-B34C-24B9E88EB74D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E04E4D8F-B6AF-AE40-ACBC-B2164A2E9A1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34380" yWindow="-3140" windowWidth="31040" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -224,9 +224,6 @@
   </si>
   <si>
     <t>Data collection start: 2019-06-01T00:00:00</t>
-  </si>
-  <si>
-    <t>Platform height is the top of the Met tower, sensor height is plaform height minus 10.8 m.</t>
   </si>
   <si>
     <t>https://github.com/heatherguy/ace-ceda-master</t>
@@ -262,6 +259,9 @@
       </rPr>
       <t>NERC Grant Award number NE/S00906X/1</t>
     </r>
+  </si>
+  <si>
+    <t>Platform height is the top of the Met tower, sensor height is plaform height minus 10.8 m. Technician log used to QC data is located here: https://github.com/heatherguy/ace-ceda-master/blob/master/qc-files/KT_bad_dates</t>
   </si>
 </sst>
 </file>
@@ -711,7 +711,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B28" sqref="B28"/>
+      <selection pane="bottomRight" activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -734,7 +734,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -822,7 +822,7 @@
         <v>14</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -940,7 +940,7 @@
         <v>30</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -972,7 +972,7 @@
         <v>36</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1000,7 +1000,7 @@
         <v>40</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
@@ -1043,7 +1043,7 @@
         <v>44</v>
       </c>
       <c r="B40" s="14" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Update KT and wind profile global and specific variables
</commit_message>
<xml_diff>
--- a/metadata/kt_metadata.xlsx
+++ b/metadata/kt_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heather/Desktop/ace-ceda-master/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E04E4D8F-B6AF-AE40-ACBC-B2164A2E9A1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B768AB77-EC9F-E646-B839-A9CA98A457EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34380" yWindow="-3140" windowWidth="31040" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="73">
   <si>
     <t>Name</t>
   </si>
@@ -191,9 +191,6 @@
   </si>
   <si>
     <t>N/a</t>
-  </si>
-  <si>
-    <t>10 second</t>
   </si>
   <si>
     <t>1 minute</t>
@@ -708,10 +705,10 @@
   <dimension ref="A1:M1003"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="223" zoomScaleNormal="223" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B40" sqref="B40"/>
+      <selection pane="bottomRight" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -734,7 +731,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -822,7 +819,7 @@
         <v>14</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -870,7 +867,7 @@
         <v>20</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -886,7 +883,7 @@
         <v>22</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -900,7 +897,7 @@
         <v>24</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -908,7 +905,7 @@
         <v>25</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -916,7 +913,7 @@
         <v>26</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -924,7 +921,7 @@
         <v>27</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -940,7 +937,7 @@
         <v>30</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -948,7 +945,7 @@
         <v>31</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -972,7 +969,7 @@
         <v>36</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1000,7 +997,7 @@
         <v>40</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
@@ -1019,7 +1016,7 @@
         <v>41</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1027,7 +1024,7 @@
         <v>42</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1035,7 +1032,7 @@
         <v>43</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1043,7 +1040,7 @@
         <v>44</v>
       </c>
       <c r="B40" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Correcting NC compliance for skin-temperature: - standard name: surface_brightness_temperature - timeSeriesPoint --> timeSeries - Added spectral range to long name and comments. - Corrected flag units to datatype 'string' - Corrected flag identifiers to datatype 'list' - Corrected flag descriptions to 'blank separated string'
</commit_message>
<xml_diff>
--- a/metadata/kt_metadata.xlsx
+++ b/metadata/kt_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10510"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heather/Desktop/ace-ceda-master/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B768AB77-EC9F-E646-B839-A9CA98A457EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D036DC35-C04B-454B-AE5B-937DA098028C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34380" yWindow="-3140" windowWidth="31040" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="global-attributes" sheetId="1" r:id="rId1"/>
@@ -160,9 +160,6 @@
     <t>v1.0</t>
   </si>
   <si>
-    <t xml:space="preserve">timeSeriesPoint </t>
-  </si>
-  <si>
     <t>KT15 Infrared Temperature sensor</t>
   </si>
   <si>
@@ -227,9 +224,6 @@
   </si>
   <si>
     <t>CF-1.6</t>
-  </si>
-  <si>
-    <t>Point measurements of snow surface temperature at Summit Station, Greenland</t>
   </si>
   <si>
     <t>72.572962N -38.470361E</t>
@@ -258,7 +252,13 @@
     </r>
   </si>
   <si>
-    <t>Platform height is the top of the Met tower, sensor height is plaform height minus 10.8 m. Technician log used to QC data is located here: https://github.com/heatherguy/ace-ceda-master/blob/master/qc-files/KT_bad_dates</t>
+    <t>timeSeries</t>
+  </si>
+  <si>
+    <t>Point measurements of snow surface brightness temperature at Summit Station, Greenland (9.6 to 11.5um spectral range)</t>
+  </si>
+  <si>
+    <t>Platform height is the top of the Met tower, sensor height is plaform height minus 10.8 m. Technician log used to QC data is located here: https://github.com/heatherguy/ace-ceda-master/blob/master/qc-files/KT_bad_dates. Spectral range of sensor is 9.6 to 11.5 um.</t>
   </si>
 </sst>
 </file>
@@ -705,10 +705,10 @@
   <dimension ref="A1:M1003"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="223" zoomScaleNormal="223" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B19" sqref="B19"/>
+      <selection pane="bottomRight" activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -731,7 +731,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -739,7 +739,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -747,7 +747,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -755,7 +755,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -771,7 +771,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -779,7 +779,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -787,7 +787,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -795,7 +795,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -803,7 +803,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -811,7 +811,7 @@
         <v>13</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -819,7 +819,7 @@
         <v>14</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -835,7 +835,7 @@
         <v>16</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -843,7 +843,7 @@
         <v>17</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -851,7 +851,7 @@
         <v>18</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -859,7 +859,7 @@
         <v>19</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -867,7 +867,7 @@
         <v>20</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -883,7 +883,7 @@
         <v>22</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -897,7 +897,7 @@
         <v>24</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -905,7 +905,7 @@
         <v>25</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -913,7 +913,7 @@
         <v>26</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -921,7 +921,7 @@
         <v>27</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -937,7 +937,7 @@
         <v>30</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -945,7 +945,7 @@
         <v>31</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -969,7 +969,7 @@
         <v>36</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -977,7 +977,7 @@
         <v>37</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -997,7 +997,7 @@
         <v>40</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
@@ -1016,7 +1016,7 @@
         <v>41</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1024,7 +1024,7 @@
         <v>42</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1032,7 +1032,7 @@
         <v>43</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>